<commit_message>
Fix : GameOver, player이동 수정
이동방향 카메라 방향으로 수정
gameOver 로직 수정
</commit_message>
<xml_diff>
--- a/Assets/Excel/Player/PlayerDB_Sheet.xlsx
+++ b/Assets/Excel/Player/PlayerDB_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Player\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\Sisyphus\Assets\Excel\Player\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F84DB3-D1AF-45B7-89F9-151E32BA8D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C1E0DE-BAB9-4C1B-91EC-8C18A1BA18D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1E85DF98-53A6-47B1-9A2F-DAF49A7487B0}"/>
+    <workbookView xWindow="945" yWindow="660" windowWidth="17520" windowHeight="15600" xr2:uid="{1E85DF98-53A6-47B1-9A2F-DAF49A7487B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>Player/Prefabs/MC01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>단단하다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>날렵하다</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -527,34 +539,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB2F3BC-9C83-4699-B76B-7A58A03E3709}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
     <col min="2" max="2" width="8.875" customWidth="1"/>
-    <col min="3" max="3" width="34.125" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="13.625" customWidth="1"/>
-    <col min="8" max="9" width="12.75" customWidth="1"/>
-    <col min="10" max="10" width="7.25" customWidth="1"/>
-    <col min="11" max="11" width="17.125" customWidth="1"/>
-    <col min="12" max="12" width="15.375" customWidth="1"/>
-    <col min="13" max="13" width="14.625" customWidth="1"/>
-    <col min="14" max="14" width="16.25" customWidth="1"/>
-    <col min="15" max="15" width="13" customWidth="1"/>
-    <col min="16" max="16" width="15.75" customWidth="1"/>
-    <col min="17" max="17" width="13.625" customWidth="1"/>
-    <col min="18" max="25" width="20.625" customWidth="1"/>
+    <col min="3" max="4" width="34.125" customWidth="1"/>
+    <col min="5" max="5" width="13.125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="10" width="12.75" customWidth="1"/>
+    <col min="11" max="11" width="7.25" customWidth="1"/>
+    <col min="12" max="12" width="17.125" customWidth="1"/>
+    <col min="13" max="13" width="15.375" customWidth="1"/>
+    <col min="14" max="14" width="14.625" customWidth="1"/>
+    <col min="15" max="15" width="16.25" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="15.75" customWidth="1"/>
+    <col min="18" max="18" width="13.625" customWidth="1"/>
+    <col min="19" max="26" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,64 +577,67 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>21234567</v>
       </c>
@@ -633,41 +648,41 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>60</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>3</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>2</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
       <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
         <v>5</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.25</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
       <c r="P2">
         <v>0</v>
       </c>
@@ -675,22 +690,25 @@
         <v>0</v>
       </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>1</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
         <v>100</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>10113011</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20000002</v>
       </c>
@@ -701,20 +719,20 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>50</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3">
         <v>0</v>
       </c>
@@ -722,39 +740,42 @@
         <v>0</v>
       </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>20</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>5</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.25</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>5</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>1</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <v>100</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>10112011</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove : ~PlayerDB 제거
</commit_message>
<xml_diff>
--- a/Assets/Excel/Player/PlayerDB_Sheet.xlsx
+++ b/Assets/Excel/Player/PlayerDB_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SpartaCoding\Sisyphus\Assets\Excel\Player\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Player\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423D7DA2-7F25-454A-ABE5-DEC34ADD7517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8B9423-0574-4D52-8623-BB40E38C77E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="26415" windowHeight="12540" xr2:uid="{1E85DF98-53A6-47B1-9A2F-DAF49A7487B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1E85DF98-53A6-47B1-9A2F-DAF49A7487B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Feat : UI 추가 및 수정
옵션 UI추가
exp 동기화
</commit_message>
<xml_diff>
--- a/Assets/Excel/Player/PlayerDB_Sheet.xlsx
+++ b/Assets/Excel/Player/PlayerDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\Sisyphus\Assets\Excel\Player\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C1E0DE-BAB9-4C1B-91EC-8C18A1BA18D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C23B84-ADCC-4A41-9904-6BF4388ECB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="660" windowWidth="17520" windowHeight="15600" xr2:uid="{1E85DF98-53A6-47B1-9A2F-DAF49A7487B0}"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="17520" windowHeight="15600" xr2:uid="{1E85DF98-53A6-47B1-9A2F-DAF49A7487B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -84,18 +84,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>LV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>maxEXP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>job</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -108,10 +96,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>startItemID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>prefabPath</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -120,10 +104,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>startInventory</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Player/Prefabs/MC01</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -137,6 +117,26 @@
   </si>
   <si>
     <t>날렵하다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_lv</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_exp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_maxEXP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_startItemID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_startInventory</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB2F3BC-9C83-4699-B76B-7A58A03E3709}">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -574,13 +574,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -595,7 +595,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>6</v>
@@ -610,7 +610,7 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>10</v>
@@ -622,19 +622,19 @@
         <v>12</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -645,10 +645,10 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -716,10 +716,10 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>

</xml_diff>